<commit_message>
Del Brand & Category and nocti error success
</commit_message>
<xml_diff>
--- a/Mobileshop/src/main/resources/templates/template.xlsx
+++ b/Mobileshop/src/main/resources/templates/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VB2\3. Ki.III\4. 77CG. Java 2\BTL\Mobileshop_SpringbootMVC_Thymeleaf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VB2\3. Ki.III\4. 77CG. Java 2\BTL\Mobileshop_SpringbootMVC_Thymeleaf\Mobileshop\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -93,7 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,16 +107,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -124,14 +136,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,118 +453,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="5">
         <v>2020</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <v>6.1</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="5">
         <v>64</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="5">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="5">
         <v>1</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="5" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add color, model, OS, Capacity template
</commit_message>
<xml_diff>
--- a/Mobileshop/src/main/resources/templates/template.xlsx
+++ b/Mobileshop/src/main/resources/templates/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VB2\3. Ki.III\4. 77CG. Java 2\BTL\Mobileshop_SpringbootMVC_Thymeleaf\Mobileshop\src\main\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VB2\7. Git Code\Mobileshop_SpringbootMVC_Thymeleaf\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
   <si>
     <t xml:space="preserve"> BrandID </t>
   </si>
@@ -69,9 +69,6 @@
     <t xml:space="preserve"> Seri </t>
   </si>
   <si>
-    <t xml:space="preserve"> Black </t>
-  </si>
-  <si>
     <t xml:space="preserve"> iphone.jpg</t>
   </si>
   <si>
@@ -151,6 +148,165 @@
   </si>
   <si>
     <t>IOS</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>OperatingSystemID</t>
+  </si>
+  <si>
+    <t>OperatingSystem</t>
+  </si>
+  <si>
+    <t>StorageCapacityID</t>
+  </si>
+  <si>
+    <t>StorageCapacity</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>ModelID</t>
+  </si>
+  <si>
+    <t>RAMID</t>
+  </si>
+  <si>
+    <t>ColorID</t>
+  </si>
+  <si>
+    <t>iphone 14-2022-128-8-Black</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S20-2020-256-8-Blue</t>
+  </si>
+  <si>
+    <t>OnePlus 9-2021-128-8-White</t>
+  </si>
+  <si>
+    <t>iphone 13-2021-256-8-Red</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S21-2021-128-8-Purple</t>
+  </si>
+  <si>
+    <t>OnePlus Nord-2020-128-6-Gray</t>
+  </si>
+  <si>
+    <t>iphone 12-2020-64-4-Black</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Note 20-2020-256-8-Bronze</t>
+  </si>
+  <si>
+    <t>OnePlus 8T-2020-128-8-Silver</t>
+  </si>
+  <si>
+    <t>iphone 11-2019-128-4-White</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S10-2019-128-8-Green</t>
+  </si>
+  <si>
+    <t>OnePlus 7 Pro-2019-256-12-Blue</t>
+  </si>
+  <si>
+    <t>iphone X-2018-256-3-Black</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Note 10-2018-256-8-Silver</t>
+  </si>
+  <si>
+    <t>OnePlus 6T-2018-128-8-Red</t>
+  </si>
+  <si>
+    <t>iphone 8-2017-64-2-Gray</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S9-2018-64-4-Blue</t>
+  </si>
+  <si>
+    <t>OnePlus 6-2018-128-6-Black</t>
+  </si>
+  <si>
+    <t>iphone 7-2016-128-2-Silver</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Note 9-2018-128-6-Blue</t>
+  </si>
+  <si>
+    <t>OnePlus 5T-2017-64-6-Red</t>
+  </si>
+  <si>
+    <t>iphone 6S-2015-32-2-Gray</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S8-2017-64-4-Gold</t>
+  </si>
+  <si>
+    <t>OnePlus 5-2017-64-6-Black</t>
+  </si>
+  <si>
+    <t>iphone 6-2014-32-2-Silver</t>
+  </si>
+  <si>
+    <t>Huawei Note 8-2017-64-6-Blue</t>
+  </si>
+  <si>
+    <t>iphone 15 pro-2016-64-6-Black</t>
+  </si>
+  <si>
+    <t>iphone SE-2016-32-2-Rose Gold</t>
+  </si>
+  <si>
+    <t>iphone 11 pro-2016-32-4-Black</t>
+  </si>
+  <si>
+    <t>OnePlus 3-2016-64-6-Silver</t>
+  </si>
+  <si>
+    <t>iPhone 15-1890-64-3-Pink</t>
+  </si>
+  <si>
+    <t>Huawie nova i5-2021-256-8-Blue</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Rose Gold</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>White</t>
   </si>
 </sst>
 </file>
@@ -523,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,19 +702,24 @@
     <col min="14" max="14" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="17" max="17" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -603,29 +764,49 @@
         <v>1</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="5" t="str">
-        <f>TRIM(CONCATENATE(TRIM(D2), "-", TRIM(F2), "-", TRIM(H2), "-", TRIM(I2), "-", TRIM(L2)))</f>
-        <v>----</v>
+      <c r="E2" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="I2" s="5">
+        <v>4</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="K2" s="6"/>
-      <c r="L2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -637,25 +818,44 @@
         <f>IFERROR(VLOOKUP(C2, Sheet3!D:E, 2, FALSE), "")</f>
         <v>1</v>
       </c>
-      <c r="R2" s="5" t="b">
+      <c r="R2" s="5">
+        <f>IFERROR(VLOOKUP(E2, Sheet3!F:G, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="S2" s="5">
+        <f>IFERROR(VLOOKUP(J2, Sheet3!H:I, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="T2" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H2, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U2" s="5">
+        <f>IFERROR(VLOOKUP(I2, Sheet3!L:M, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="V2" s="5">
+        <f>IFERROR(VLOOKUP(L2, Sheet3!N:O, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="W2" s="5" t="b">
         <f>IF(ISBLANK(O2), TRUE, FALSE)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="5" t="str">
-        <f t="shared" ref="E3:E29" si="0">TRIM(CONCATENATE(TRIM(D3), "-", TRIM(F3), "-", TRIM(H3), "-", TRIM(I3), "-", TRIM(L3)))</f>
-        <v>Huawie nova i5-2021-256-8-Blue</v>
+        <v>34</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="F3" s="5">
         <v>2021</v>
@@ -664,26 +864,26 @@
         <v>6.4</v>
       </c>
       <c r="H3" s="5">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="I3" s="5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5">
         <v>1</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P3" s="5">
         <f>IFERROR(VLOOKUP(B3, Sheet3!B:C, 2, FALSE), "")</f>
@@ -693,26 +893,43 @@
         <f>IFERROR(VLOOKUP(C3, Sheet3!D:E, 2, FALSE), "")</f>
         <v>1</v>
       </c>
-      <c r="R3" s="5" t="b">
-        <f t="shared" ref="R3:R29" si="1">IF(ISBLANK(O3), TRUE, FALSE)</f>
+      <c r="R3" s="5">
+        <f>IFERROR(VLOOKUP(E3, Sheet3!F:G, 2, FALSE), "")</f>
+        <v>6</v>
+      </c>
+      <c r="S3" s="5">
+        <f>IFERROR(VLOOKUP(J3, Sheet3!H:I, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="T3" s="5">
+        <f>IFERROR(VLOOKUP(H3, Sheet3!J:K, 2, FALSE), "")</f>
+        <v>4</v>
+      </c>
+      <c r="U3" s="5">
+        <f>IFERROR(VLOOKUP(I3, Sheet3!L:M, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="V3" s="5">
+        <f>IFERROR(VLOOKUP(L3, Sheet3!N:O, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="W3" s="5" t="b">
+        <f t="shared" ref="W3:W29" si="0">IF(ISBLANK(O3), TRUE, FALSE)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>iPhone X-2020-64-4-Black</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="5">
         <v>2020</v>
       </c>
@@ -720,28 +937,28 @@
         <v>6.1</v>
       </c>
       <c r="H4" s="5">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="I4" s="5">
         <v>4</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="N4" s="5">
-        <v>1</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="P4" s="5">
         <f>IFERROR(VLOOKUP(B4, Sheet3!B:C, 2, FALSE), "")</f>
@@ -751,25 +968,44 @@
         <f>IFERROR(VLOOKUP(C4, Sheet3!D:E, 2, FALSE), "")</f>
         <v>1</v>
       </c>
-      <c r="R4" s="5" t="b">
-        <f t="shared" si="1"/>
+      <c r="R4" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E4, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S4" s="5">
+        <f>IFERROR(VLOOKUP(J4, Sheet3!H:I, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="T4" s="5">
+        <f>IFERROR(VLOOKUP(H4, Sheet3!J:K, 2, FALSE), "")</f>
+        <v>6</v>
+      </c>
+      <c r="U4" s="5">
+        <f>IFERROR(VLOOKUP(I4, Sheet3!L:M, 2, FALSE), "")</f>
+        <v>2</v>
+      </c>
+      <c r="V4" s="5">
+        <f>IFERROR(VLOOKUP(L4, Sheet3!N:O, 2, FALSE), "")</f>
+        <v>4</v>
+      </c>
+      <c r="W4" s="5" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="J5" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="K5" s="6"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -783,20 +1019,37 @@
         <f>IFERROR(VLOOKUP(C5, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R5" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E5, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S5" s="5">
+        <f>IFERROR(VLOOKUP(J5, Sheet3!H:I, 2, FALSE), "")</f>
+        <v>1</v>
+      </c>
+      <c r="T5" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H5, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U5" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I5, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V5" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L5, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W5" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -815,20 +1068,37 @@
         <f>IFERROR(VLOOKUP(C6, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R6" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E6, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S6" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J6, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T6" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H6, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U6" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I6, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V6" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L6, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W6" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -847,20 +1117,37 @@
         <f>IFERROR(VLOOKUP(C7, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R7" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R7" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E7, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S7" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J7, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T7" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H7, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U7" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I7, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V7" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L7, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W7" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -879,20 +1166,37 @@
         <f>IFERROR(VLOOKUP(C8, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R8" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R8" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E8, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S8" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J8, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T8" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H8, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U8" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I8, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V8" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L8, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W8" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
@@ -911,20 +1215,37 @@
         <f>IFERROR(VLOOKUP(C9, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R9" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E9, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S9" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J9, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T9" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H9, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U9" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I9, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V9" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L9, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W9" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -943,20 +1264,37 @@
         <f>IFERROR(VLOOKUP(C10, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R10" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E10, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S10" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J10, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T10" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H10, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U10" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I10, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V10" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L10, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W10" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -975,20 +1313,37 @@
         <f>IFERROR(VLOOKUP(C11, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R11" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R11" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E11, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S11" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J11, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T11" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H11, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U11" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I11, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V11" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L11, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W11" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -1007,20 +1362,37 @@
         <f>IFERROR(VLOOKUP(C12, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R12" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R12" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E12, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S12" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J12, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T12" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H12, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U12" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I12, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V12" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L12, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W12" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -1039,20 +1411,37 @@
         <f>IFERROR(VLOOKUP(C13, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R13" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R13" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E13, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S13" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J13, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T13" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H13, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U13" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I13, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V13" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L13, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W13" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1071,20 +1460,37 @@
         <f>IFERROR(VLOOKUP(C14, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R14" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R14" s="5" t="str">
+        <f>IFERROR(VLOOKUP(E14, Sheet3!F:G, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="S14" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J14, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T14" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H14, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U14" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I14, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V14" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L14, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W14" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1103,20 +1509,34 @@
         <f>IFERROR(VLOOKUP(C15, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R15" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R15" s="5"/>
+      <c r="S15" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J15, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T15" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H15, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U15" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I15, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V15" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L15, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W15" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1135,20 +1555,34 @@
         <f>IFERROR(VLOOKUP(C16, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R16" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R16" s="5"/>
+      <c r="S16" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J16, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T16" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H16, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U16" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I16, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V16" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L16, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W16" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1167,20 +1601,34 @@
         <f>IFERROR(VLOOKUP(C17, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R17" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R17" s="5"/>
+      <c r="S17" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J17, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T17" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H17, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U17" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I17, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V17" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L17, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W17" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -1199,20 +1647,34 @@
         <f>IFERROR(VLOOKUP(C18, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R18" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R18" s="5"/>
+      <c r="S18" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J18, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T18" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H18, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U18" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I18, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V18" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L18, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W18" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1231,20 +1693,34 @@
         <f>IFERROR(VLOOKUP(C19, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R19" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R19" s="5"/>
+      <c r="S19" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J19, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T19" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H19, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U19" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I19, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V19" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L19, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W19" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1263,20 +1739,34 @@
         <f>IFERROR(VLOOKUP(C20, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R20" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R20" s="5"/>
+      <c r="S20" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J20, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T20" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H20, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U20" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I20, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V20" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L20, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W20" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1295,20 +1785,34 @@
         <f>IFERROR(VLOOKUP(C21, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R21" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R21" s="5"/>
+      <c r="S21" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J21, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T21" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H21, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U21" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I21, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V21" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L21, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W21" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1327,20 +1831,34 @@
         <f>IFERROR(VLOOKUP(C22, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R22" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R22" s="5"/>
+      <c r="S22" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J22, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T22" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H22, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U22" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I22, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V22" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L22, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W22" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -1359,20 +1877,34 @@
         <f>IFERROR(VLOOKUP(C23, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R23" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R23" s="5"/>
+      <c r="S23" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J23, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T23" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H23, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U23" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I23, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V23" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L23, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W23" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -1391,20 +1923,34 @@
         <f>IFERROR(VLOOKUP(C24, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R24" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R24" s="5"/>
+      <c r="S24" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J24, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T24" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H24, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U24" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I24, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V24" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L24, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W24" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -1423,20 +1969,34 @@
         <f>IFERROR(VLOOKUP(C25, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R25" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R25" s="5"/>
+      <c r="S25" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J25, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T25" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H25, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U25" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I25, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V25" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L25, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W25" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -1455,20 +2015,34 @@
         <f>IFERROR(VLOOKUP(C26, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R26" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R26" s="5"/>
+      <c r="S26" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J26, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T26" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H26, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U26" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I26, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V26" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L26, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W26" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -1487,20 +2061,34 @@
         <f>IFERROR(VLOOKUP(C27, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R27" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R27" s="5"/>
+      <c r="S27" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J27, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T27" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H27, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U27" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I27, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V27" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L27, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W27" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -1519,20 +2107,34 @@
         <f>IFERROR(VLOOKUP(C28, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R28" s="5" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R28" s="5"/>
+      <c r="S28" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J28, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T28" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H28, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U28" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I28, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V28" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L28, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W28" s="5" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>----</v>
-      </c>
+      <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -1551,8 +2153,25 @@
         <f>IFERROR(VLOOKUP(C29, Sheet3!D:E, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="R29" s="5" t="b">
-        <f t="shared" si="1"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5" t="str">
+        <f>IFERROR(VLOOKUP(J29, Sheet3!H:I, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="T29" s="5" t="str">
+        <f>IFERROR(VLOOKUP(H29, Sheet3!J:K, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="U29" s="5" t="str">
+        <f>IFERROR(VLOOKUP(I29, Sheet3!L:M, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="V29" s="5" t="str">
+        <f>IFERROR(VLOOKUP(L29, Sheet3!N:O, 2, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="W29" s="5" t="b">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1561,7 +2180,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet3!$B$2:$B$7</xm:f>
@@ -1574,6 +2193,36 @@
           </x14:formula1>
           <xm:sqref>C2:C29</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet3!$F$2:$F$609</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet3!$H$2:$H$34</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet3!$L$2:$L$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet3!$N$2:$N$300</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet3!$J$2:$J$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H29</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1582,111 +2231,567 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E9"/>
+  <dimension ref="B1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="C3" s="7">
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>32</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>64</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>84</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="7">
         <v>4</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>128</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
+        <v>85</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="7">
         <v>5</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>256</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>12</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="7"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>512</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>16</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>87</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>1024</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="M8">
+        <v>7</v>
+      </c>
+      <c r="N8" t="s">
+        <v>88</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>2048</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>32</v>
+      </c>
+      <c r="M9">
+        <v>8</v>
+      </c>
+      <c r="N9" t="s">
+        <v>89</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="N10" t="s">
+        <v>90</v>
+      </c>
+      <c r="O10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="N11" t="s">
+        <v>91</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="N12" t="s">
+        <v>92</v>
+      </c>
+      <c r="O12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="N13" t="s">
+        <v>93</v>
+      </c>
+      <c r="O13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>